<commit_message>
minor change (warning message if not-implemented) added to xl_read_heatexchanger.py
</commit_message>
<xml_diff>
--- a/carbatpy/heat_exchanger_input0.xlsx
+++ b/carbatpy/heat_exchanger_input0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atakan\sciebo\Python\carbatpy\carbatpy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D4EB8EA-C7DA-471A-A990-FACE3BFB5709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88D4F05C-A6B7-4729-AE4F-033B537DBACF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11460" activeTab="1" xr2:uid="{4E6C26D7-6C6E-4333-9A67-A60B9315F33E}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11460" xr2:uid="{4E6C26D7-6C6E-4333-9A67-A60B9315F33E}"/>
   </bookViews>
   <sheets>
     <sheet name="Geometry" sheetId="1" r:id="rId1"/>
@@ -553,8 +553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8E9C067-F795-4212-A253-B3A1494FB4F8}">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -781,7 +781,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A01BE42C-B3CE-4C88-976A-3493C0B4F75D}">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -1094,10 +1094,13 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="A2" sqref="A2:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="1" max="1" width="23.81640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
Excel parameter readinand input is moved to heat_exchanger.py, excel-input file modified. The run script has to be modified
</commit_message>
<xml_diff>
--- a/carbatpy/heat_exchanger_input0.xlsx
+++ b/carbatpy/heat_exchanger_input0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atakan\sciebo\Python\carbatpy\carbatpy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88D4F05C-A6B7-4729-AE4F-033B537DBACF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CCF6D749-EB92-46E3-82C3-4AC00A884F30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11460" xr2:uid="{4E6C26D7-6C6E-4333-9A67-A60B9315F33E}"/>
+    <workbookView xWindow="60525" yWindow="2850" windowWidth="14400" windowHeight="8190" xr2:uid="{4E6C26D7-6C6E-4333-9A67-A60B9315F33E}"/>
   </bookViews>
   <sheets>
     <sheet name="Geometry" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="57">
   <si>
     <t>props</t>
   </si>
@@ -75,15 +75,9 @@
     <t>Water</t>
   </si>
   <si>
-    <t>variable name</t>
-  </si>
-  <si>
     <t>unit</t>
   </si>
   <si>
-    <t>comment/choice</t>
-  </si>
-  <si>
     <t>fixed</t>
   </si>
   <si>
@@ -96,9 +90,6 @@
     <t>p_in</t>
   </si>
   <si>
-    <t>variable</t>
-  </si>
-  <si>
     <t>value</t>
   </si>
   <si>
@@ -108,9 +99,6 @@
     <t>comment</t>
   </si>
   <si>
-    <t>value choices</t>
-  </si>
-  <si>
     <t>value_1</t>
   </si>
   <si>
@@ -132,9 +120,6 @@
     <t>W/ m2 / K</t>
   </si>
   <si>
-    <t>value 2</t>
-  </si>
-  <si>
     <t>wall_thickness</t>
   </si>
   <si>
@@ -168,24 +153,12 @@
     <t>mole fraction</t>
   </si>
   <si>
-    <t>fixed 1</t>
-  </si>
-  <si>
-    <t>fixed 2</t>
-  </si>
-  <si>
     <t>output</t>
   </si>
   <si>
-    <t>problem</t>
-  </si>
-  <si>
     <t>calculation_type</t>
   </si>
   <si>
-    <t>thermal comductivity</t>
-  </si>
-  <si>
     <t>W / m / K</t>
   </si>
   <si>
@@ -199,6 +172,42 @@
   </si>
   <si>
     <t>T_ref</t>
+  </si>
+  <si>
+    <t>option</t>
+  </si>
+  <si>
+    <t>thermal_conductivity</t>
+  </si>
+  <si>
+    <t>variable_name</t>
+  </si>
+  <si>
+    <t>value_2</t>
+  </si>
+  <si>
+    <t>fixed_1</t>
+  </si>
+  <si>
+    <t>fixed_2</t>
+  </si>
+  <si>
+    <t>value_choices</t>
+  </si>
+  <si>
+    <t>unused</t>
+  </si>
+  <si>
+    <t>configuration</t>
+  </si>
+  <si>
+    <t>Fluid_1</t>
+  </si>
+  <si>
+    <t>constant</t>
+  </si>
+  <si>
+    <t>Name of Sheet for the selection of 1 or two fluids,or  value_2: constant or T-slope</t>
   </si>
 </sst>
 </file>
@@ -551,10 +560,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8E9C067-F795-4212-A253-B3A1494FB4F8}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:I11"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -562,48 +574,51 @@
     <col min="1" max="1" width="28.2265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" t="s">
+      <c r="G1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A3" t="s">
         <v>24</v>
       </c>
-      <c r="C1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.75">
-      <c r="A2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.75">
-      <c r="A3" t="s">
-        <v>28</v>
-      </c>
       <c r="B3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.75">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B4">
         <v>500</v>
@@ -612,16 +627,16 @@
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
-      </c>
-      <c r="I4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.75">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -632,13 +647,13 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.75">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -649,16 +664,16 @@
         <v>0.08</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E6" t="s">
-        <v>16</v>
-      </c>
-      <c r="I6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -666,18 +681,18 @@
         <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E7" t="s">
-        <v>16</v>
-      </c>
-      <c r="I7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B8" s="1">
         <v>1E-3</v>
@@ -686,18 +701,18 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="D8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E8" t="s">
-        <v>16</v>
-      </c>
-      <c r="I8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B9">
         <v>800</v>
@@ -706,18 +721,18 @@
         <v>800</v>
       </c>
       <c r="D9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E9" t="s">
-        <v>16</v>
-      </c>
-      <c r="I9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.75">
+        <v>14</v>
+      </c>
+      <c r="F9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B10" s="1">
         <v>8000</v>
@@ -726,38 +741,38 @@
         <v>8000</v>
       </c>
       <c r="D10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E10" t="s">
-        <v>16</v>
-      </c>
-      <c r="I10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.75">
+        <v>14</v>
+      </c>
+      <c r="F10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E11" t="s">
-        <v>16</v>
-      </c>
-      <c r="I11" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.75">
+        <v>14</v>
+      </c>
+      <c r="F11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B12" s="1">
         <v>16</v>
@@ -766,10 +781,24 @@
         <v>16</v>
       </c>
       <c r="D12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E12" t="s">
-        <v>16</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" t="s">
+        <v>55</v>
+      </c>
+      <c r="H13" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -782,38 +811,44 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="G1" sqref="G1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="1" max="1" width="16.6328125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I1" t="s">
         <v>19</v>
       </c>
-      <c r="B1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" t="s">
-        <v>22</v>
-      </c>
       <c r="J1" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.75">
@@ -826,7 +861,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -846,13 +881,13 @@
         <v>0.8</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F4" t="s">
         <v>9</v>
       </c>
-      <c r="H4" t="s">
-        <v>42</v>
+      <c r="G4" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.75">
@@ -869,18 +904,18 @@
         <v>0.9</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F5" t="s">
         <v>10</v>
       </c>
-      <c r="H5" t="s">
-        <v>42</v>
+      <c r="G5" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B6">
         <v>350</v>
@@ -892,15 +927,15 @@
         <v>370</v>
       </c>
       <c r="E6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B7" s="1">
         <v>1000000</v>
@@ -912,15 +947,15 @@
         <v>2000000</v>
       </c>
       <c r="E7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7" t="s">
-        <v>21</v>
+        <v>14</v>
+      </c>
+      <c r="G7" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B8">
         <v>1.2E-2</v>
@@ -931,8 +966,8 @@
       <c r="D8">
         <v>0.02</v>
       </c>
-      <c r="H8" t="s">
-        <v>26</v>
+      <c r="G8" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -945,38 +980,41 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I1" t="s">
         <v>19</v>
       </c>
-      <c r="B1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" t="s">
-        <v>22</v>
-      </c>
       <c r="J1" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.75">
@@ -989,7 +1027,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -1009,18 +1047,18 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F4" t="s">
         <v>11</v>
       </c>
-      <c r="H4" t="s">
-        <v>42</v>
+      <c r="G4" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B5">
         <v>350</v>
@@ -1032,15 +1070,15 @@
         <v>370</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" t="s">
-        <v>6</v>
+        <v>14</v>
+      </c>
+      <c r="G5" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B6" s="1">
         <v>1000000</v>
@@ -1052,15 +1090,15 @@
         <v>2000000</v>
       </c>
       <c r="E6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H6" t="s">
-        <v>21</v>
+        <v>14</v>
+      </c>
+      <c r="G6" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B7">
         <v>1.2E-2</v>
@@ -1071,8 +1109,13 @@
       <c r="D7">
         <v>0.02</v>
       </c>
-      <c r="H7" t="s">
-        <v>26</v>
+      <c r="G7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="G8" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.75">
@@ -1091,10 +1134,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A56B6A2-0CAF-4DED-8F52-E833FCDF80DB}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B3"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -1102,39 +1145,54 @@
     <col min="1" max="1" width="23.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C1" t="s">
-        <v>31</v>
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="G1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.75">
+        <v>45</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.75">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="B3">
         <v>283.14999999999998</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>